<commit_message>
Create Testing Units for CEMI Case
</commit_message>
<xml_diff>
--- a/CEMI_chapas.xlsx
+++ b/CEMI_chapas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56367\Documents\GitHub\PyFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F861305-453E-424A-9976-F23E174A76B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976D7180-3E5C-421C-9106-E16926FD24A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19103" yWindow="-98" windowWidth="19395" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19103" yWindow="-98" windowWidth="19395" windowHeight="11475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MBOM" sheetId="2" r:id="rId1"/>
@@ -668,7 +668,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -708,7 +708,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7692789-1C38-476F-B78A-11B6D05AE770}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1052,7 +1052,7 @@
         <v>210.8</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1130,7 +1130,7 @@
         <v>210.8</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1208,7 +1208,7 @@
         <v>418.40000000000003</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1286,7 +1286,7 @@
         <v>436</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1312,7 +1312,7 @@
         <v>507.59999999999997</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1390,7 +1390,7 @@
         <v>168.79999999999998</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1468,7 +1468,7 @@
         <v>316.8</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1520,7 +1520,7 @@
         <v>513.19999999999993</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1598,7 +1598,7 @@
         <v>487.6</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1676,7 +1676,7 @@
         <v>507.59999999999997</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1728,7 +1728,7 @@
         <v>417.6</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1754,7 +1754,7 @@
         <v>418.40000000000003</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -1806,7 +1806,7 @@
         <v>232.79999999999998</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1832,7 +1832,7 @@
         <v>310.39999999999998</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -1988,7 +1988,7 @@
         <v>176.8</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2014,7 +2014,7 @@
         <v>210.8</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -2066,7 +2066,7 @@
         <v>210.8</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -2092,7 +2092,7 @@
         <v>232.79999999999998</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -2118,7 +2118,7 @@
         <v>168.79999999999998</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -2144,7 +2144,7 @@
         <v>308.39999999999998</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -2222,7 +2222,7 @@
         <v>428.8</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -2300,7 +2300,7 @@
         <v>417.6</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -2404,7 +2404,7 @@
         <v>487.2</v>
       </c>
       <c r="H54">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -2456,7 +2456,7 @@
         <v>210.8</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -2482,7 +2482,7 @@
         <v>310.39999999999998</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
@@ -2508,7 +2508,7 @@
         <v>428.8</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
@@ -2586,7 +2586,7 @@
         <v>428.8</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
@@ -2638,7 +2638,7 @@
         <v>487.2</v>
       </c>
       <c r="H63">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
@@ -2664,7 +2664,7 @@
         <v>317.60000000000002</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
@@ -2716,7 +2716,7 @@
         <v>232.79999999999998</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
@@ -2768,7 +2768,7 @@
         <v>168.79999999999998</v>
       </c>
       <c r="H68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
@@ -2794,7 +2794,7 @@
         <v>428.8</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
@@ -2820,7 +2820,7 @@
         <v>316</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
@@ -2898,7 +2898,7 @@
         <v>428.8</v>
       </c>
       <c r="H73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
@@ -2976,7 +2976,7 @@
         <v>317.60000000000002</v>
       </c>
       <c r="H76">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
@@ -3002,7 +3002,7 @@
         <v>514</v>
       </c>
       <c r="H77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
@@ -3054,7 +3054,7 @@
         <v>441.2</v>
       </c>
       <c r="H79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
@@ -3080,7 +3080,7 @@
         <v>436</v>
       </c>
       <c r="H80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
@@ -3106,7 +3106,7 @@
         <v>507.59999999999997</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
@@ -3158,7 +3158,7 @@
         <v>493.59999999999997</v>
       </c>
       <c r="H83">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
@@ -3210,7 +3210,7 @@
         <v>176.8</v>
       </c>
       <c r="H85">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
@@ -3236,7 +3236,7 @@
         <v>442.40000000000003</v>
       </c>
       <c r="H86">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
@@ -3262,7 +3262,7 @@
         <v>514</v>
       </c>
       <c r="H87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
@@ -3314,7 +3314,7 @@
         <v>513.19999999999993</v>
       </c>
       <c r="H89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
@@ -3340,7 +3340,7 @@
         <v>310.39999999999998</v>
       </c>
       <c r="H90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
@@ -3366,7 +3366,7 @@
         <v>316</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3379,8 +3379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF013EF5-E4A9-4708-8857-50220345B45D}">
   <dimension ref="A1:Q96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L75" sqref="L75:M75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:M92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B33" ca="1" si="0">RAND()</f>
-        <v>0.52849124398362268</v>
+        <v>0.1424598366512807</v>
       </c>
       <c r="E2" t="s">
         <v>205</v>
@@ -3426,7 +3426,7 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45455905603338953</v>
+        <v>0.49283574532492047</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -3455,13 +3455,8 @@
       <c r="M3">
         <v>34</v>
       </c>
-      <c r="P3" s="2">
-        <v>3.7060185185185182E-3</v>
-      </c>
-      <c r="Q3" s="1">
-        <f>5*60+20</f>
-        <v>320</v>
-      </c>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -3469,7 +3464,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62506290719153479</v>
+        <v>0.83195004726672728</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -3498,9 +3493,7 @@
       <c r="M4">
         <v>62</v>
       </c>
-      <c r="P4" s="2">
-        <v>1.2662037037037038E-3</v>
-      </c>
+      <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -3508,7 +3501,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26428241897444993</v>
+        <v>0.76831342667723901</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -3537,9 +3530,7 @@
       <c r="M5">
         <v>71</v>
       </c>
-      <c r="P5" s="2">
-        <v>2.9837962962962965E-3</v>
-      </c>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -3547,7 +3538,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54207488829696804</v>
+        <v>0.27015878855966657</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -3576,9 +3567,7 @@
       <c r="M6">
         <v>69</v>
       </c>
-      <c r="P6" s="2">
-        <v>1.2939814814814815E-3</v>
-      </c>
+      <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -3586,7 +3575,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21960860225548851</v>
+        <v>0.922483352938399</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -3615,9 +3604,7 @@
       <c r="M7">
         <v>26</v>
       </c>
-      <c r="P7" s="2">
-        <v>2.5277777777777777E-3</v>
-      </c>
+      <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -3625,7 +3612,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.35511364010046642</v>
+        <v>0.46099181251853871</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -3654,9 +3641,7 @@
       <c r="M8">
         <v>47</v>
       </c>
-      <c r="P8" s="2">
-        <v>1.3935185185185185E-3</v>
-      </c>
+      <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -3664,7 +3649,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8603575161872961E-3</v>
+        <v>0.18794754078420595</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -3693,9 +3678,7 @@
       <c r="M9">
         <v>12</v>
       </c>
-      <c r="P9" s="2">
-        <v>8.6157407407407398E-3</v>
-      </c>
+      <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -3703,7 +3686,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29653506788372253</v>
+        <v>0.69720406562093129</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -3732,9 +3715,7 @@
       <c r="M10">
         <v>25</v>
       </c>
-      <c r="P10" s="2">
-        <v>3.0208333333333333E-3</v>
-      </c>
+      <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -3742,7 +3723,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94390618111362701</v>
+        <v>0.787158795827402</v>
       </c>
       <c r="E11">
         <v>9</v>
@@ -3771,9 +3752,7 @@
       <c r="M11">
         <v>32</v>
       </c>
-      <c r="P11" s="2">
-        <v>2.5277777777777777E-3</v>
-      </c>
+      <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -3781,7 +3760,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89582218568215877</v>
+        <v>0.26771400533884171</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -3810,9 +3789,7 @@
       <c r="M12">
         <v>66</v>
       </c>
-      <c r="P12" s="2">
-        <v>2.5995370370370369E-3</v>
-      </c>
+      <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -3820,7 +3797,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76451819387242304</v>
+        <v>0.76128226941511701</v>
       </c>
       <c r="E13">
         <v>11</v>
@@ -3849,9 +3826,7 @@
       <c r="M13">
         <v>44</v>
       </c>
-      <c r="P13" s="2">
-        <v>1.0231481481481482E-3</v>
-      </c>
+      <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -3859,7 +3834,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73328741502284067</v>
+        <v>0.80578827328983427</v>
       </c>
       <c r="E14">
         <v>12</v>
@@ -3888,9 +3863,7 @@
       <c r="M14">
         <v>23</v>
       </c>
-      <c r="P14" s="2">
-        <v>2.4675925925925924E-3</v>
-      </c>
+      <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -3898,7 +3871,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15882477819997221</v>
+        <v>0.78200918196127467</v>
       </c>
       <c r="E15">
         <v>13</v>
@@ -3927,9 +3900,7 @@
       <c r="M15">
         <v>58</v>
       </c>
-      <c r="P15" s="2">
-        <v>1.8796296296296297E-3</v>
-      </c>
+      <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -3937,7 +3908,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8316522734562746E-2</v>
+        <v>0.44147983557145209</v>
       </c>
       <c r="E16">
         <v>14</v>
@@ -3966,9 +3937,7 @@
       <c r="M16">
         <v>29</v>
       </c>
-      <c r="P16" s="2">
-        <v>2.5277777777777777E-3</v>
-      </c>
+      <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -3976,7 +3945,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.22904665843400129</v>
+        <v>0.23061733776068782</v>
       </c>
       <c r="E17">
         <v>15</v>
@@ -4005,9 +3974,7 @@
       <c r="M17">
         <v>84</v>
       </c>
-      <c r="P17" s="2">
-        <v>2.5995370370370369E-3</v>
-      </c>
+      <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -4015,7 +3982,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96429261326491367</v>
+        <v>0.66456118761450245</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -4044,9 +4011,7 @@
       <c r="M18">
         <v>18</v>
       </c>
-      <c r="P18" s="2">
-        <v>2.9837962962962965E-3</v>
-      </c>
+      <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -4054,7 +4019,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99315327738587467</v>
+        <v>0.19522335347984576</v>
       </c>
       <c r="E19">
         <v>17</v>
@@ -4083,9 +4048,7 @@
       <c r="M19">
         <v>76</v>
       </c>
-      <c r="P19" s="2">
-        <v>1.3935185185185185E-3</v>
-      </c>
+      <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -4093,7 +4056,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7792074287939319E-2</v>
+        <v>0.11912282334701341</v>
       </c>
       <c r="E20">
         <v>18</v>
@@ -4122,9 +4085,7 @@
       <c r="M20">
         <v>43</v>
       </c>
-      <c r="P20" s="2">
-        <v>2.4629629629629632E-3</v>
-      </c>
+      <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -4132,7 +4093,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6836989276804326E-2</v>
+        <v>0.12978227565129652</v>
       </c>
       <c r="E21">
         <v>19</v>
@@ -4161,9 +4122,7 @@
       <c r="M21">
         <v>22</v>
       </c>
-      <c r="P21" s="2">
-        <v>1.2662037037037038E-3</v>
-      </c>
+      <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -4171,7 +4130,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32263020293294453</v>
+        <v>0.25381539172167433</v>
       </c>
       <c r="E22">
         <v>20</v>
@@ -4200,9 +4159,7 @@
       <c r="M22">
         <v>7</v>
       </c>
-      <c r="P22" s="2">
-        <v>2.5277777777777777E-3</v>
-      </c>
+      <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -4210,7 +4167,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68340159434575443</v>
+        <v>0.27088264225703795</v>
       </c>
       <c r="E23">
         <v>21</v>
@@ -4239,9 +4196,7 @@
       <c r="M23">
         <v>27</v>
       </c>
-      <c r="P23" s="2">
-        <v>1.8310185185185183E-3</v>
-      </c>
+      <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -4249,7 +4204,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66062961832831846</v>
+        <v>0.32485194429843955</v>
       </c>
       <c r="E24">
         <v>22</v>
@@ -4278,9 +4233,7 @@
       <c r="M24">
         <v>87</v>
       </c>
-      <c r="P24" s="2">
-        <v>3.0162037037037041E-3</v>
-      </c>
+      <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -4288,7 +4241,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6756706191754076E-2</v>
+        <v>0.333703865426209</v>
       </c>
       <c r="E25">
         <v>23</v>
@@ -4317,9 +4270,7 @@
       <c r="M25">
         <v>89</v>
       </c>
-      <c r="P25" s="2">
-        <v>2.9768518518518516E-3</v>
-      </c>
+      <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -4327,7 +4278,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44072818497618316</v>
+        <v>0.63493112757490233</v>
       </c>
       <c r="E26">
         <v>24</v>
@@ -4356,9 +4307,7 @@
       <c r="M26">
         <v>13</v>
       </c>
-      <c r="P26" s="2">
-        <v>2.5277777777777777E-3</v>
-      </c>
+      <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -4366,7 +4315,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4710547903203578</v>
+        <v>0.73923899657837322</v>
       </c>
       <c r="E27">
         <v>25</v>
@@ -4395,9 +4344,7 @@
       <c r="M27">
         <v>75</v>
       </c>
-      <c r="P27" s="2">
-        <v>2.4675925925925924E-3</v>
-      </c>
+      <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
@@ -4405,7 +4352,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9463166714134217E-2</v>
+        <v>0.70306778952122051</v>
       </c>
       <c r="E28">
         <v>26</v>
@@ -4434,9 +4381,7 @@
       <c r="M28">
         <v>80</v>
       </c>
-      <c r="P28" s="2">
-        <v>2.6064814814814813E-3</v>
-      </c>
+      <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
@@ -4444,7 +4389,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50044364093278637</v>
+        <v>0.11376812855818896</v>
       </c>
       <c r="E29">
         <v>27</v>
@@ -4473,9 +4418,7 @@
       <c r="M29">
         <v>74</v>
       </c>
-      <c r="P29" s="2">
-        <v>1.8796296296296297E-3</v>
-      </c>
+      <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
@@ -4483,7 +4426,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40123647084048197</v>
+        <v>9.6369805588970237E-2</v>
       </c>
       <c r="E30">
         <v>28</v>
@@ -4512,9 +4455,7 @@
       <c r="M30">
         <v>85</v>
       </c>
-      <c r="P30" s="2">
-        <v>2.5277777777777777E-3</v>
-      </c>
+      <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
@@ -4522,7 +4463,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79161866856389385</v>
+        <v>0.14412480774078895</v>
       </c>
       <c r="E31">
         <v>29</v>
@@ -4551,9 +4492,7 @@
       <c r="M31">
         <v>11</v>
       </c>
-      <c r="P31" s="2">
-        <v>1.0231481481481482E-3</v>
-      </c>
+      <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
@@ -4561,7 +4500,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51015968366785058</v>
+        <v>0.39268145595364379</v>
       </c>
       <c r="E32">
         <v>30</v>
@@ -4590,9 +4529,7 @@
       <c r="M32">
         <v>68</v>
       </c>
-      <c r="P32" s="2">
-        <v>8.6157407407407398E-3</v>
-      </c>
+      <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
@@ -4600,7 +4537,7 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52864006957522558</v>
+        <v>0.88102655391835671</v>
       </c>
       <c r="E33">
         <v>31</v>
@@ -4629,9 +4566,7 @@
       <c r="M33">
         <v>73</v>
       </c>
-      <c r="P33" s="2">
-        <v>1.8310185185185183E-3</v>
-      </c>
+      <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34">
@@ -4639,7 +4574,7 @@
       </c>
       <c r="B34">
         <f t="shared" ref="B34:B65" ca="1" si="1">RAND()</f>
-        <v>0.55092524355555339</v>
+        <v>0.88573006706937851</v>
       </c>
       <c r="E34">
         <v>32</v>
@@ -4668,9 +4603,7 @@
       <c r="M34">
         <v>21</v>
       </c>
-      <c r="P34" s="2">
-        <v>1.2939814814814815E-3</v>
-      </c>
+      <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35">
@@ -4678,7 +4611,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67591094797358675</v>
+        <v>0.83804202140799267</v>
       </c>
       <c r="E35">
         <v>33</v>
@@ -4707,9 +4640,7 @@
       <c r="M35">
         <v>55</v>
       </c>
-      <c r="P35" s="2">
-        <v>1.2939814814814815E-3</v>
-      </c>
+      <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36">
@@ -4717,7 +4648,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24424291205218995</v>
+        <v>0.70794128957977454</v>
       </c>
       <c r="E36">
         <v>34</v>
@@ -4746,9 +4677,7 @@
       <c r="M36">
         <v>88</v>
       </c>
-      <c r="P36" s="2">
-        <v>1.2662037037037038E-3</v>
-      </c>
+      <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37">
@@ -4756,7 +4685,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38214265697463623</v>
+        <v>0.99603738536492703</v>
       </c>
       <c r="E37">
         <v>35</v>
@@ -4785,9 +4714,7 @@
       <c r="M37">
         <v>40</v>
       </c>
-      <c r="P37" s="2">
-        <v>2.4629629629629632E-3</v>
-      </c>
+      <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38">
@@ -4795,7 +4722,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.83837302591591101</v>
+        <v>0.72708578241692712</v>
       </c>
       <c r="E38">
         <v>36</v>
@@ -4824,9 +4751,7 @@
       <c r="M38">
         <v>33</v>
       </c>
-      <c r="P38" s="2">
-        <v>1.8425925925925925E-3</v>
-      </c>
+      <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39">
@@ -4834,7 +4759,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.79416419380296843</v>
+        <v>0.11766354720595462</v>
       </c>
       <c r="E39">
         <v>37</v>
@@ -4863,9 +4788,7 @@
       <c r="M39">
         <v>56</v>
       </c>
-      <c r="P39" s="2">
-        <v>1.8749999999999999E-3</v>
-      </c>
+      <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40">
@@ -4873,7 +4796,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1179255716410927E-2</v>
+        <v>0.31825087796640594</v>
       </c>
       <c r="E40">
         <v>38</v>
@@ -4902,9 +4825,7 @@
       <c r="M40">
         <v>2</v>
       </c>
-      <c r="P40" s="2">
-        <v>1.2939814814814815E-3</v>
-      </c>
+      <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41">
@@ -4912,7 +4833,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55019039395886116</v>
+        <v>0.98480624032353692</v>
       </c>
       <c r="E41">
         <v>39</v>
@@ -4941,9 +4862,7 @@
       <c r="M41">
         <v>4</v>
       </c>
-      <c r="P41" s="2">
-        <v>1.3935185185185185E-3</v>
-      </c>
+      <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42">
@@ -4951,7 +4870,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.40397773214188493</v>
+        <v>0.71143823408686258</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -4980,9 +4899,7 @@
       <c r="M42">
         <v>19</v>
       </c>
-      <c r="P42" s="2">
-        <v>5.5324074074074078E-3</v>
-      </c>
+      <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43">
@@ -4990,7 +4907,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30767324895629478</v>
+        <v>0.76524545797173815</v>
       </c>
       <c r="E43">
         <v>41</v>
@@ -5019,9 +4936,7 @@
       <c r="M43">
         <v>17</v>
       </c>
-      <c r="P43" s="2">
-        <v>1.0694444444444445E-3</v>
-      </c>
+      <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44">
@@ -5029,7 +4944,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10838647817120994</v>
+        <v>0.98385278171649893</v>
       </c>
       <c r="E44">
         <v>42</v>
@@ -5058,9 +4973,7 @@
       <c r="M44">
         <v>64</v>
       </c>
-      <c r="P44" s="2">
-        <v>1.8310185185185183E-3</v>
-      </c>
+      <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45">
@@ -5068,7 +4981,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67907288011240863</v>
+        <v>0.75783957368284816</v>
       </c>
       <c r="E45">
         <v>43</v>
@@ -5097,9 +5010,7 @@
       <c r="M45">
         <v>31</v>
       </c>
-      <c r="P45" s="2">
-        <v>2.6064814814814813E-3</v>
-      </c>
+      <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46">
@@ -5107,7 +5018,7 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="1"/>
-        <v>6.7486454088438785E-2</v>
+        <v>0.86704055373469713</v>
       </c>
       <c r="E46">
         <v>44</v>
@@ -5136,9 +5047,7 @@
       <c r="M46">
         <v>9</v>
       </c>
-      <c r="P46" s="2">
-        <v>2.9837962962962965E-3</v>
-      </c>
+      <c r="P46" s="2"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47">
@@ -5146,7 +5055,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97604773616853879</v>
+        <v>0.94894393080747308</v>
       </c>
       <c r="E47">
         <v>45</v>
@@ -5175,9 +5084,7 @@
       <c r="M47">
         <v>50</v>
       </c>
-      <c r="P47" s="2">
-        <v>5.4351851851851853E-3</v>
-      </c>
+      <c r="P47" s="2"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48">
@@ -5185,7 +5092,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28804206292044721</v>
+        <v>0.67551126993402788</v>
       </c>
       <c r="E48">
         <v>46</v>
@@ -5214,9 +5121,7 @@
       <c r="M48">
         <v>5</v>
       </c>
-      <c r="P48" s="2">
-        <v>3.7893518518518515E-3</v>
-      </c>
+      <c r="P48" s="2"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49">
@@ -5224,7 +5129,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46724905494941815</v>
+        <v>0.10610313800581461</v>
       </c>
       <c r="E49">
         <v>47</v>
@@ -5253,9 +5158,7 @@
       <c r="M49">
         <v>46</v>
       </c>
-      <c r="P49" s="2">
-        <v>1.8842592592592594E-3</v>
-      </c>
+      <c r="P49" s="2"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50">
@@ -5263,7 +5166,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33143208244714595</v>
+        <v>0.73893609823562711</v>
       </c>
       <c r="E50">
         <v>48</v>
@@ -5292,9 +5195,7 @@
       <c r="M50">
         <v>78</v>
       </c>
-      <c r="P50" s="2">
-        <v>2.5277777777777777E-3</v>
-      </c>
+      <c r="P50" s="2"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51">
@@ -5302,7 +5203,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8210574685736598</v>
+        <v>0.66884650455817485</v>
       </c>
       <c r="E51">
         <v>49</v>
@@ -5331,9 +5232,7 @@
       <c r="M51">
         <v>35</v>
       </c>
-      <c r="P51" s="2">
-        <v>2.5694444444444445E-3</v>
-      </c>
+      <c r="P51" s="2"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52">
@@ -5341,7 +5240,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41453329541544637</v>
+        <v>0.19514823622294331</v>
       </c>
       <c r="E52">
         <v>50</v>
@@ -5370,9 +5269,7 @@
       <c r="M52">
         <v>63</v>
       </c>
-      <c r="P52" s="2">
-        <v>3.0208333333333333E-3</v>
-      </c>
+      <c r="P52" s="2"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53">
@@ -5380,7 +5277,7 @@
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12476764116877415</v>
+        <v>4.9022148934937504E-2</v>
       </c>
       <c r="E53">
         <v>51</v>
@@ -5409,9 +5306,7 @@
       <c r="M53">
         <v>61</v>
       </c>
-      <c r="P53" s="2">
-        <v>1.8749999999999999E-3</v>
-      </c>
+      <c r="P53" s="2"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54">
@@ -5419,7 +5314,7 @@
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30035575103809786</v>
+        <v>0.90746840800843354</v>
       </c>
       <c r="E54">
         <v>52</v>
@@ -5448,9 +5343,7 @@
       <c r="M54">
         <v>77</v>
       </c>
-      <c r="P54" s="2">
-        <v>2.5694444444444445E-3</v>
-      </c>
+      <c r="P54" s="2"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55">
@@ -5458,7 +5351,7 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92051224727049674</v>
+        <v>0.36692806487946283</v>
       </c>
       <c r="E55">
         <v>53</v>
@@ -5487,9 +5380,7 @@
       <c r="M55">
         <v>54</v>
       </c>
-      <c r="P55" s="2">
-        <v>1.8749999999999999E-3</v>
-      </c>
+      <c r="P55" s="2"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56">
@@ -5497,7 +5388,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23248558861351709</v>
+        <v>0.43370653341947996</v>
       </c>
       <c r="E56">
         <v>54</v>
@@ -5526,9 +5417,7 @@
       <c r="M56">
         <v>67</v>
       </c>
-      <c r="P56" s="2">
-        <v>2.8657407407407407E-3</v>
-      </c>
+      <c r="P56" s="2"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57">
@@ -5536,7 +5425,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23026731609892603</v>
+        <v>0.96622705887188309</v>
       </c>
       <c r="E57">
         <v>55</v>
@@ -5565,9 +5454,7 @@
       <c r="M57">
         <v>83</v>
       </c>
-      <c r="P57" s="2">
-        <v>3.7893518518518515E-3</v>
-      </c>
+      <c r="P57" s="2"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58">
@@ -5575,7 +5462,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49039478803934033</v>
+        <v>4.2974723660077929E-2</v>
       </c>
       <c r="E58">
         <v>56</v>
@@ -5604,9 +5491,7 @@
       <c r="M58">
         <v>36</v>
       </c>
-      <c r="P58" s="2">
-        <v>1.0694444444444445E-3</v>
-      </c>
+      <c r="P58" s="2"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59">
@@ -5614,7 +5499,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
-        <v>0.54967420638001319</v>
+        <v>7.7445419812100069E-2</v>
       </c>
       <c r="E59">
         <v>57</v>
@@ -5643,9 +5528,7 @@
       <c r="M59">
         <v>48</v>
       </c>
-      <c r="P59" s="2">
-        <v>1.8749999999999999E-3</v>
-      </c>
+      <c r="P59" s="2"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60">
@@ -5653,7 +5536,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>0.40967068687541019</v>
+        <v>0.81769977411547201</v>
       </c>
       <c r="E60">
         <v>58</v>
@@ -5682,9 +5565,7 @@
       <c r="M60">
         <v>6</v>
       </c>
-      <c r="P60" s="2">
-        <v>4.0879629629629625E-3</v>
-      </c>
+      <c r="P60" s="2"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61">
@@ -5692,7 +5573,7 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="1"/>
-        <v>0.88807160032316723</v>
+        <v>0.85159537724487722</v>
       </c>
       <c r="E61">
         <v>59</v>
@@ -5721,9 +5602,7 @@
       <c r="M61">
         <v>16</v>
       </c>
-      <c r="P61" s="2">
-        <v>3.0162037037037041E-3</v>
-      </c>
+      <c r="P61" s="2"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62">
@@ -5731,7 +5610,7 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26287500247868589</v>
+        <v>0.62355923591200202</v>
       </c>
       <c r="E62">
         <v>60</v>
@@ -5760,9 +5639,7 @@
       <c r="M62">
         <v>14</v>
       </c>
-      <c r="P62" s="2">
-        <v>3.0162037037037041E-3</v>
-      </c>
+      <c r="P62" s="2"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63">
@@ -5770,7 +5647,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87996023576895821</v>
+        <v>0.36334129792222092</v>
       </c>
       <c r="E63">
         <v>61</v>
@@ -5799,9 +5676,7 @@
       <c r="M63">
         <v>53</v>
       </c>
-      <c r="P63" s="2">
-        <v>2.8680555555555555E-3</v>
-      </c>
+      <c r="P63" s="2"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64">
@@ -5809,7 +5684,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="1"/>
-        <v>0.83163207028931163</v>
+        <v>0.89685485408119803</v>
       </c>
       <c r="E64">
         <v>62</v>
@@ -5838,9 +5713,7 @@
       <c r="M64">
         <v>65</v>
       </c>
-      <c r="P64" s="2">
-        <v>2.8657407407407407E-3</v>
-      </c>
+      <c r="P64" s="2"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65">
@@ -5848,7 +5721,7 @@
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="1"/>
-        <v>8.3586265310783392E-2</v>
+        <v>0.59825644361398367</v>
       </c>
       <c r="E65">
         <v>63</v>
@@ -5877,9 +5750,7 @@
       <c r="M65">
         <v>81</v>
       </c>
-      <c r="P65" s="2">
-        <v>7.4907407407407414E-3</v>
-      </c>
+      <c r="P65" s="2"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66">
@@ -5887,7 +5758,7 @@
       </c>
       <c r="B66">
         <f t="shared" ref="B66:B91" ca="1" si="2">RAND()</f>
-        <v>0.53637392184219945</v>
+        <v>0.17143642599323827</v>
       </c>
       <c r="E66">
         <v>64</v>
@@ -5916,9 +5787,7 @@
       <c r="M66">
         <v>59</v>
       </c>
-      <c r="P66" s="2">
-        <v>1.0231481481481482E-3</v>
-      </c>
+      <c r="P66" s="2"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67">
@@ -5926,7 +5795,7 @@
       </c>
       <c r="B67">
         <f t="shared" ca="1" si="2"/>
-        <v>0.95591962616200332</v>
+        <v>0.87467709960849094</v>
       </c>
       <c r="E67">
         <v>65</v>
@@ -5955,9 +5824,7 @@
       <c r="M67">
         <v>39</v>
       </c>
-      <c r="P67" s="2">
-        <v>2.8657407407407407E-3</v>
-      </c>
+      <c r="P67" s="2"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68">
@@ -5965,7 +5832,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="2"/>
-        <v>0.22674398484700276</v>
+        <v>0.63099169406948175</v>
       </c>
       <c r="E68">
         <v>66</v>
@@ -5994,9 +5861,7 @@
       <c r="M68">
         <v>49</v>
       </c>
-      <c r="P68" s="2">
-        <v>2.5694444444444445E-3</v>
-      </c>
+      <c r="P68" s="2"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69">
@@ -6004,7 +5869,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="2"/>
-        <v>6.3735791173192946E-2</v>
+        <v>0.14918541593083567</v>
       </c>
       <c r="E69">
         <v>67</v>
@@ -6033,9 +5898,7 @@
       <c r="M69">
         <v>79</v>
       </c>
-      <c r="P69" s="2">
-        <v>3.1157407407407405E-3</v>
-      </c>
+      <c r="P69" s="2"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70">
@@ -6043,7 +5906,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="2"/>
-        <v>4.1556953906641936E-2</v>
+        <v>0.50658718949192039</v>
       </c>
       <c r="E70">
         <v>68</v>
@@ -6072,9 +5935,7 @@
       <c r="M70">
         <v>20</v>
       </c>
-      <c r="P70" s="2">
-        <v>1.3935185185185185E-3</v>
-      </c>
+      <c r="P70" s="2"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71">
@@ -6082,7 +5943,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="2"/>
-        <v>0.84504686811476282</v>
+        <v>0.99582664044093971</v>
       </c>
       <c r="E71">
         <v>69</v>
@@ -6111,9 +5972,7 @@
       <c r="M71">
         <v>37</v>
       </c>
-      <c r="P71" s="2">
-        <v>1.2662037037037038E-3</v>
-      </c>
+      <c r="P71" s="2"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72">
@@ -6121,7 +5980,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="2"/>
-        <v>0.96845329022210569</v>
+        <v>0.91396466842163715</v>
       </c>
       <c r="E72">
         <v>70</v>
@@ -6150,9 +6009,7 @@
       <c r="M72">
         <v>24</v>
       </c>
-      <c r="P72" s="2">
-        <v>1.8842592592592594E-3</v>
-      </c>
+      <c r="P72" s="2"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73">
@@ -6160,7 +6017,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="2"/>
-        <v>0.23279678375741364</v>
+        <v>0.52505381800105788</v>
       </c>
       <c r="E73">
         <v>71</v>
@@ -6189,9 +6046,7 @@
       <c r="M73">
         <v>30</v>
       </c>
-      <c r="P73" s="2">
-        <v>1.3935185185185185E-3</v>
-      </c>
+      <c r="P73" s="2"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74">
@@ -6199,7 +6054,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="2"/>
-        <v>0.10759274874762603</v>
+        <v>0.7563311827837268</v>
       </c>
       <c r="E74">
         <v>72</v>
@@ -6228,9 +6083,7 @@
       <c r="M74">
         <v>28</v>
       </c>
-      <c r="P74" s="2">
-        <v>3.0208333333333333E-3</v>
-      </c>
+      <c r="P74" s="2"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75">
@@ -6238,7 +6091,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="2"/>
-        <v>0.17566092462667293</v>
+        <v>0.72271176669188752</v>
       </c>
       <c r="E75">
         <v>73</v>
@@ -6267,9 +6120,7 @@
       <c r="M75">
         <v>1</v>
       </c>
-      <c r="P75" s="2">
-        <v>1.8425925925925925E-3</v>
-      </c>
+      <c r="P75" s="2"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76">
@@ -6277,7 +6128,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="2"/>
-        <v>0.27078652251806656</v>
+        <v>0.48885915620589748</v>
       </c>
       <c r="E76">
         <v>74</v>
@@ -6306,9 +6157,7 @@
       <c r="M76">
         <v>57</v>
       </c>
-      <c r="P76" s="2">
-        <v>2.4629629629629632E-3</v>
-      </c>
+      <c r="P76" s="2"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77">
@@ -6316,7 +6165,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="2"/>
-        <v>0.35714582934603711</v>
+        <v>0.15382179151149633</v>
       </c>
       <c r="E77">
         <v>75</v>
@@ -6345,9 +6194,7 @@
       <c r="M77">
         <v>70</v>
       </c>
-      <c r="P77" s="2">
-        <v>2.9837962962962965E-3</v>
-      </c>
+      <c r="P77" s="2"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78">
@@ -6355,7 +6202,7 @@
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88269297311337125</v>
+        <v>0.60307904676978674</v>
       </c>
       <c r="E78">
         <v>76</v>
@@ -6384,9 +6231,7 @@
       <c r="M78">
         <v>72</v>
       </c>
-      <c r="P78" s="2">
-        <v>1.8796296296296297E-3</v>
-      </c>
+      <c r="P78" s="2"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79">
@@ -6394,7 +6239,7 @@
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="2"/>
-        <v>0.24777463927422871</v>
+        <v>0.9657884637222871</v>
       </c>
       <c r="E79">
         <v>77</v>
@@ -6423,9 +6268,7 @@
       <c r="M79">
         <v>42</v>
       </c>
-      <c r="P79" s="2">
-        <v>2.9837962962962965E-3</v>
-      </c>
+      <c r="P79" s="2"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80">
@@ -6433,7 +6276,7 @@
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="2"/>
-        <v>0.26311493826603427</v>
+        <v>0.86797879208076345</v>
       </c>
       <c r="E80">
         <v>78</v>
@@ -6462,9 +6305,7 @@
       <c r="M80">
         <v>10</v>
       </c>
-      <c r="P80" s="2">
-        <v>2.9768518518518516E-3</v>
-      </c>
+      <c r="P80" s="2"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81">
@@ -6472,7 +6313,7 @@
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="2"/>
-        <v>0.24941026625974005</v>
+        <v>0.52035348717863383</v>
       </c>
       <c r="E81">
         <v>79</v>
@@ -6501,9 +6342,7 @@
       <c r="M81">
         <v>52</v>
       </c>
-      <c r="P81" s="2">
-        <v>1.0231481481481482E-3</v>
-      </c>
+      <c r="P81" s="2"/>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82">
@@ -6511,7 +6350,7 @@
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="2"/>
-        <v>0.22888899665688556</v>
+        <v>0.73350418694128272</v>
       </c>
       <c r="E82">
         <v>80</v>
@@ -6540,9 +6379,7 @@
       <c r="M82">
         <v>3</v>
       </c>
-      <c r="P82" s="2">
-        <v>2.9837962962962965E-3</v>
-      </c>
+      <c r="P82" s="2"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83">
@@ -6550,7 +6387,7 @@
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="2"/>
-        <v>0.90254245774449515</v>
+        <v>0.97357664950600264</v>
       </c>
       <c r="E83">
         <v>81</v>
@@ -6579,9 +6416,7 @@
       <c r="M83">
         <v>15</v>
       </c>
-      <c r="P83" s="2">
-        <v>1.8842592592592594E-3</v>
-      </c>
+      <c r="P83" s="2"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84">
@@ -6589,7 +6424,7 @@
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5896140447086426E-2</v>
+        <v>0.87305580639126945</v>
       </c>
       <c r="E84">
         <v>82</v>
@@ -6618,9 +6453,7 @@
       <c r="M84">
         <v>86</v>
       </c>
-      <c r="P84" s="2">
-        <v>2.6064814814814813E-3</v>
-      </c>
+      <c r="P84" s="2"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85">
@@ -6628,7 +6461,7 @@
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="2"/>
-        <v>0.72710420309722468</v>
+        <v>0.90140305918852159</v>
       </c>
       <c r="E85">
         <v>83</v>
@@ -6657,9 +6490,7 @@
       <c r="M85">
         <v>90</v>
       </c>
-      <c r="P85" s="2">
-        <v>1.2662037037037038E-3</v>
-      </c>
+      <c r="P85" s="2"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86">
@@ -6667,7 +6498,7 @@
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="2"/>
-        <v>0.49749215925658563</v>
+        <v>0.7471435408466589</v>
       </c>
       <c r="E86">
         <v>84</v>
@@ -6696,9 +6527,7 @@
       <c r="M86">
         <v>41</v>
       </c>
-      <c r="P86" s="2">
-        <v>2.8680555555555555E-3</v>
-      </c>
+      <c r="P86" s="2"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87">
@@ -6706,7 +6535,7 @@
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87064420488094929</v>
+        <v>0.66122024816389247</v>
       </c>
       <c r="E87">
         <v>85</v>
@@ -6735,9 +6564,7 @@
       <c r="M87">
         <v>82</v>
       </c>
-      <c r="P87" s="2">
-        <v>7.3101851851851852E-3</v>
-      </c>
+      <c r="P87" s="2"/>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88">
@@ -6745,7 +6572,7 @@
       </c>
       <c r="B88">
         <f t="shared" ca="1" si="2"/>
-        <v>0.76474133826088053</v>
+        <v>0.30854178139420807</v>
       </c>
       <c r="E88">
         <v>86</v>
@@ -6774,9 +6601,7 @@
       <c r="M88">
         <v>8</v>
       </c>
-      <c r="P88" s="2">
-        <v>8.6157407407407398E-3</v>
-      </c>
+      <c r="P88" s="2"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89">
@@ -6784,7 +6609,7 @@
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="2"/>
-        <v>0.44286474273712817</v>
+        <v>0.87819509462827983</v>
       </c>
       <c r="E89">
         <v>87</v>
@@ -6813,9 +6638,7 @@
       <c r="M89">
         <v>38</v>
       </c>
-      <c r="P89" s="2">
-        <v>2.8680555555555555E-3</v>
-      </c>
+      <c r="P89" s="2"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90">
@@ -6823,7 +6646,7 @@
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="2"/>
-        <v>8.724569270060889E-2</v>
+        <v>0.74293265602820269</v>
       </c>
       <c r="E90">
         <v>88</v>
@@ -6852,9 +6675,7 @@
       <c r="M90">
         <v>60</v>
       </c>
-      <c r="P90" s="2">
-        <v>2.5995370370370369E-3</v>
-      </c>
+      <c r="P90" s="2"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91">
@@ -6862,7 +6683,7 @@
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="2"/>
-        <v>2.8221626416258361E-2</v>
+        <v>0.61503754750965989</v>
       </c>
       <c r="E91">
         <v>89</v>
@@ -6891,9 +6712,7 @@
       <c r="M91">
         <v>45</v>
       </c>
-      <c r="P91" s="2">
-        <v>5.5324074074074078E-3</v>
-      </c>
+      <c r="P91" s="2"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E92">
@@ -6923,9 +6742,7 @@
       <c r="M92">
         <v>51</v>
       </c>
-      <c r="P92" s="2">
-        <v>7.4907407407407414E-3</v>
-      </c>
+      <c r="P92" s="2"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F94" t="s">
@@ -6985,6 +6802,7 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>